<commit_message>
Sound! Score is displayed when winning and losing a round! Startup string! Sound switches on and off using the Go button at start!
All but 12 bytes of code space used.
</commit_message>
<xml_diff>
--- a/code/display_calculator.xlsx
+++ b/code/display_calculator.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
   <si>
     <t>A</t>
   </si>
@@ -99,13 +99,22 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +124,14 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -142,9 +159,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A09D22-8E6A-4619-91AF-6B05C1AEA697}">
-  <dimension ref="B1:O29"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="R24" sqref="R24:R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,16 +500,13 @@
     <col min="1" max="3" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1">
-        <v>1</v>
-      </c>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1">
         <f>B1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1">
         <v>64</v>
@@ -511,9 +527,12 @@
         <f>K20</f>
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C2">
+      <c r="R1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
@@ -521,7 +540,7 @@
       </c>
       <c r="F2" s="1">
         <f>C2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -533,7 +552,7 @@
         <v>245</v>
       </c>
       <c r="K2" t="str">
-        <f>DEC2HEX(J2)</f>
+        <f t="shared" ref="K2:K32" si="0">DEC2HEX(J2)</f>
         <v>F5</v>
       </c>
       <c r="N2" t="s">
@@ -543,8 +562,14 @@
         <f>K21</f>
         <v>A6</v>
       </c>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
@@ -562,11 +587,17 @@
         <v>5</v>
       </c>
       <c r="K3" t="str">
-        <f>DEC2HEX(J3)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
       <c r="C4">
         <v>1</v>
       </c>
@@ -587,7 +618,7 @@
         <v>227</v>
       </c>
       <c r="K4" t="str">
-        <f>DEC2HEX(J4)</f>
+        <f t="shared" si="0"/>
         <v>E3</v>
       </c>
       <c r="N4" t="s">
@@ -597,14 +628,17 @@
         <f>K23</f>
         <v>77</v>
       </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="1">
         <f>A4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>128</v>
@@ -616,7 +650,7 @@
         <v>103</v>
       </c>
       <c r="K5" t="str">
-        <f>DEC2HEX(J5)</f>
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
       <c r="N5" t="s">
@@ -626,14 +660,21 @@
         <f>K12</f>
         <v>D7</v>
       </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q5" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" t="str">
+        <f>K30</f>
+        <v>B6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="1">
         <f>A2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>16</v>
@@ -645,7 +686,7 @@
         <v>23</v>
       </c>
       <c r="K6" t="str">
-        <f>DEC2HEX(J6)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="N6" t="s">
@@ -655,14 +696,21 @@
         <f>K22</f>
         <v>C6</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6" t="str">
+        <f>K28</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="1">
         <f>B3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -674,7 +722,7 @@
         <v>118</v>
       </c>
       <c r="K7" t="str">
-        <f>DEC2HEX(J7)</f>
+        <f t="shared" si="0"/>
         <v>76</v>
       </c>
       <c r="N7" t="s">
@@ -684,8 +732,15 @@
         <f>K16</f>
         <v>F2</v>
       </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R7" t="str">
+        <f>K20</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I8">
         <v>6</v>
       </c>
@@ -693,17 +748,24 @@
         <v>246</v>
       </c>
       <c r="K8" t="str">
-        <f>DEC2HEX(J8)</f>
+        <f t="shared" si="0"/>
         <v>F6</v>
       </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R8" t="str">
+        <f>K12</f>
+        <v>D7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>9</v>
       </c>
       <c r="F9">
         <f>SUMPRODUCT(F1:F7,G1:G7)</f>
-        <v>69</v>
+        <v>150</v>
       </c>
       <c r="I9">
         <v>7</v>
@@ -712,7 +774,7 @@
         <v>69</v>
       </c>
       <c r="K9" t="str">
-        <f>DEC2HEX(J9)</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="N9" t="s">
@@ -722,8 +784,15 @@
         <f>K24</f>
         <v>F5</v>
       </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R9" t="str">
+        <f>K26</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I10">
         <v>8</v>
       </c>
@@ -731,7 +800,7 @@
         <v>247</v>
       </c>
       <c r="K10" t="str">
-        <f>DEC2HEX(J10)</f>
+        <f t="shared" si="0"/>
         <v>F7</v>
       </c>
       <c r="N10" t="s">
@@ -741,8 +810,15 @@
         <f>K25</f>
         <v>B5</v>
       </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R10" t="str">
+        <f>K19</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I11">
         <v>9</v>
       </c>
@@ -750,7 +826,7 @@
         <v>119</v>
       </c>
       <c r="K11" t="str">
-        <f>DEC2HEX(J11)</f>
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="N11" t="s">
@@ -760,8 +836,11 @@
         <f>K16</f>
         <v>F2</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I12" t="s">
         <v>0</v>
       </c>
@@ -769,7 +848,7 @@
         <v>215</v>
       </c>
       <c r="K12" t="str">
-        <f>DEC2HEX(J12)</f>
+        <f t="shared" si="0"/>
         <v>D7</v>
       </c>
       <c r="N12" t="s">
@@ -779,8 +858,15 @@
         <f>K26</f>
         <v>82</v>
       </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q12" t="s">
+        <v>19</v>
+      </c>
+      <c r="R12" t="str">
+        <f>K23</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
         <v>1</v>
       </c>
@@ -788,11 +874,18 @@
         <v>182</v>
       </c>
       <c r="K13" t="str">
-        <f>DEC2HEX(J13)</f>
+        <f t="shared" si="0"/>
         <v>B6</v>
       </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" t="str">
+        <f>K12</f>
+        <v>D7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I14" t="s">
         <v>2</v>
       </c>
@@ -800,7 +893,7 @@
         <v>240</v>
       </c>
       <c r="K14" t="str">
-        <f>DEC2HEX(J14)</f>
+        <f t="shared" si="0"/>
         <v>F0</v>
       </c>
       <c r="N14" t="s">
@@ -810,8 +903,15 @@
         <f>K23</f>
         <v>77</v>
       </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q14" t="s">
+        <v>18</v>
+      </c>
+      <c r="R14" t="str">
+        <f>K22</f>
+        <v>C6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I15" t="s">
         <v>3</v>
       </c>
@@ -819,7 +919,7 @@
         <v>167</v>
       </c>
       <c r="K15" t="str">
-        <f>DEC2HEX(J15)</f>
+        <f t="shared" si="0"/>
         <v>A7</v>
       </c>
       <c r="N15" t="s">
@@ -829,8 +929,15 @@
         <f>K21</f>
         <v>A6</v>
       </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q15" t="s">
+        <v>4</v>
+      </c>
+      <c r="R15" t="str">
+        <f>K16</f>
+        <v>F2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I16" t="s">
         <v>4</v>
       </c>
@@ -838,7 +945,7 @@
         <v>242</v>
       </c>
       <c r="K16" t="str">
-        <f>DEC2HEX(J16)</f>
+        <f t="shared" si="0"/>
         <v>F2</v>
       </c>
       <c r="N16" t="s">
@@ -848,8 +955,11 @@
         <f>K27</f>
         <v>C3</v>
       </c>
-    </row>
-    <row r="17" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I17" t="s">
         <v>5</v>
       </c>
@@ -857,11 +967,18 @@
         <v>210</v>
       </c>
       <c r="K17" t="str">
-        <f>DEC2HEX(J17)</f>
+        <f t="shared" si="0"/>
         <v>D2</v>
       </c>
-    </row>
-    <row r="18" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="Q17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R17" t="str">
+        <f>K31</f>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="18" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I18" t="s">
         <v>11</v>
       </c>
@@ -869,7 +986,7 @@
         <v>151</v>
       </c>
       <c r="K18" t="str">
-        <f>DEC2HEX(J18)</f>
+        <f t="shared" si="0"/>
         <v>97</v>
       </c>
       <c r="N18" t="s">
@@ -879,8 +996,15 @@
         <f>K19</f>
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18" t="str">
+        <f>K2</f>
+        <v>F5</v>
+      </c>
+    </row>
+    <row r="19" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
         <v>12</v>
       </c>
@@ -888,7 +1012,7 @@
         <v>55</v>
       </c>
       <c r="K19" t="str">
-        <f>DEC2HEX(J19)</f>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="N19" t="s">
@@ -898,8 +1022,11 @@
         <f>K16</f>
         <v>F2</v>
       </c>
-    </row>
-    <row r="20" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="R19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I20" t="s">
         <v>16</v>
       </c>
@@ -907,7 +1034,7 @@
         <v>134</v>
       </c>
       <c r="K20" t="str">
-        <f>DEC2HEX(J20)</f>
+        <f t="shared" si="0"/>
         <v>86</v>
       </c>
       <c r="N20" t="s">
@@ -917,8 +1044,11 @@
         <f>K7</f>
         <v>76</v>
       </c>
-    </row>
-    <row r="21" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="R20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
         <v>17</v>
       </c>
@@ -926,11 +1056,14 @@
         <v>166</v>
       </c>
       <c r="K21" t="str">
-        <f>DEC2HEX(J21)</f>
+        <f t="shared" si="0"/>
         <v>A6</v>
       </c>
-    </row>
-    <row r="22" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="R21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
         <v>18</v>
       </c>
@@ -938,7 +1071,7 @@
         <v>198</v>
       </c>
       <c r="K22" t="str">
-        <f>DEC2HEX(J22)</f>
+        <f t="shared" si="0"/>
         <v>C6</v>
       </c>
       <c r="N22" t="s">
@@ -948,8 +1081,11 @@
         <f>K29</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="R22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
         <v>19</v>
       </c>
@@ -957,7 +1093,7 @@
         <v>119</v>
       </c>
       <c r="K23" t="str">
-        <f>DEC2HEX(J23)</f>
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="N23" t="s">
@@ -968,7 +1104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
         <v>15</v>
       </c>
@@ -976,7 +1112,7 @@
         <v>245</v>
       </c>
       <c r="K24" t="str">
-        <f>DEC2HEX(J24)</f>
+        <f t="shared" si="0"/>
         <v>F5</v>
       </c>
       <c r="N24" t="s">
@@ -986,8 +1122,15 @@
         <f>K22</f>
         <v>C6</v>
       </c>
-    </row>
-    <row r="25" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="Q24" t="s">
+        <v>15</v>
+      </c>
+      <c r="R24" t="str">
+        <f>K24</f>
+        <v>F5</v>
+      </c>
+    </row>
+    <row r="25" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I25" t="s">
         <v>20</v>
       </c>
@@ -995,7 +1138,7 @@
         <v>181</v>
       </c>
       <c r="K25" t="str">
-        <f>DEC2HEX(J25)</f>
+        <f t="shared" si="0"/>
         <v>B5</v>
       </c>
       <c r="N25" t="s">
@@ -1005,8 +1148,15 @@
         <f>K16</f>
         <v>F2</v>
       </c>
-    </row>
-    <row r="26" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="Q25" t="s">
+        <v>5</v>
+      </c>
+      <c r="R25" t="str">
+        <f>K17</f>
+        <v>D2</v>
+      </c>
+    </row>
+    <row r="26" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I26" t="s">
         <v>21</v>
       </c>
@@ -1014,11 +1164,18 @@
         <v>130</v>
       </c>
       <c r="K26" t="str">
-        <f>DEC2HEX(J26)</f>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="27" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="Q26" t="s">
+        <v>5</v>
+      </c>
+      <c r="R26" t="str">
+        <f>K17</f>
+        <v>D2</v>
+      </c>
+    </row>
+    <row r="27" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I27" t="s">
         <v>22</v>
       </c>
@@ -1026,11 +1183,11 @@
         <v>195</v>
       </c>
       <c r="K27" t="str">
-        <f>DEC2HEX(J27)</f>
+        <f t="shared" si="0"/>
         <v>C3</v>
       </c>
     </row>
-    <row r="28" spans="9:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I28" t="s">
         <v>24</v>
       </c>
@@ -1038,11 +1195,18 @@
         <v>5</v>
       </c>
       <c r="K28" t="str">
-        <f>DEC2HEX(J28)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="Q28" t="s">
+        <v>15</v>
+      </c>
+      <c r="R28" t="str">
+        <f>K24</f>
+        <v>F5</v>
+      </c>
+    </row>
+    <row r="29" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I29" t="s">
         <v>23</v>
       </c>
@@ -1050,8 +1214,52 @@
         <v>69</v>
       </c>
       <c r="K29" t="str">
-        <f>DEC2HEX(J29)</f>
+        <f t="shared" si="0"/>
         <v>45</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>16</v>
+      </c>
+      <c r="R29" t="str">
+        <f>K20</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="9:18" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>25</v>
+      </c>
+      <c r="J30">
+        <v>182</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="0"/>
+        <v>B6</v>
+      </c>
+    </row>
+    <row r="31" spans="9:18" x14ac:dyDescent="0.25">
+      <c r="I31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J31">
+        <f>5+8</f>
+        <v>13</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="32" spans="9:18" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>27</v>
+      </c>
+      <c r="J32">
+        <v>150</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="0"/>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>